<commit_message>
Added percent gaps to this table, now to remove from main text
</commit_message>
<xml_diff>
--- a/Manuscript/Revision/TableS3.xlsx
+++ b/Manuscript/Revision/TableS3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="2660" windowWidth="25360" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="-33300" yWindow="440" windowWidth="25360" windowHeight="15240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>HA</t>
   </si>
   <si>
-    <t>FUBAR</t>
-  </si>
-  <si>
-    <t>PAML</t>
-  </si>
-  <si>
     <t>GP41</t>
   </si>
   <si>
@@ -39,9 +33,6 @@
     <t>Number of Taxa</t>
   </si>
   <si>
-    <t>Inference Method</t>
-  </si>
-  <si>
     <t>Average Percent MSA Sites Masked (Average Number of Residues Masked)</t>
   </si>
   <si>
@@ -57,157 +48,163 @@
     <t>BMweightsP</t>
   </si>
   <si>
-    <t>0.01% (43.25)</t>
-  </si>
-  <si>
-    <t>0.01% (42.49)</t>
-  </si>
-  <si>
-    <t>0.01% (44.35)</t>
-  </si>
-  <si>
-    <t>0.02% (89.32)</t>
-  </si>
-  <si>
-    <t>0.02% (87.69)</t>
-  </si>
-  <si>
-    <t>0.026% (113.67)</t>
-  </si>
-  <si>
-    <t>0.01% (107.75)</t>
-  </si>
-  <si>
-    <t>0.01% (106.73)</t>
-  </si>
-  <si>
-    <t>0.01% (108.67)</t>
-  </si>
-  <si>
-    <t>0.025% (256.84)</t>
-  </si>
-  <si>
-    <t>0.024% (251.01)</t>
-  </si>
-  <si>
-    <t>0.026% (264.28)</t>
-  </si>
-  <si>
-    <t>0.027% (653.38)</t>
-  </si>
-  <si>
-    <t>0.026% (634.76)</t>
-  </si>
-  <si>
-    <t>0.032% (762.93)</t>
-  </si>
-  <si>
-    <t>0.094% (2280.15)</t>
-  </si>
-  <si>
-    <t>0.096% (2326.67)</t>
-  </si>
-  <si>
-    <t>0.104% (2522.89)</t>
-  </si>
-  <si>
-    <t>0.006% (382.88)</t>
-  </si>
-  <si>
-    <t>0.006% (366.12)</t>
-  </si>
-  <si>
-    <t>0.006% (413.73)</t>
-  </si>
-  <si>
-    <t>0.018% (1126.08)</t>
-  </si>
-  <si>
-    <t>0.019% (1198.67)</t>
-  </si>
-  <si>
-    <t>0.019% (1245.29)</t>
-  </si>
-  <si>
-    <t>0.009% (40.56)</t>
-  </si>
-  <si>
-    <t>0.009% (40.01)</t>
-  </si>
-  <si>
-    <t>0.009% (41.82)</t>
-  </si>
-  <si>
-    <t>0.021% (93.1)</t>
-  </si>
-  <si>
-    <t>0.021% (91.96)</t>
-  </si>
-  <si>
-    <t>0.027% (117.72)</t>
-  </si>
-  <si>
-    <t>0.014% (143.81)</t>
-  </si>
-  <si>
-    <t>0.014% (141.86)</t>
-  </si>
-  <si>
-    <t>0.014% (148.7)</t>
-  </si>
-  <si>
-    <t>0.042% (435.8)</t>
-  </si>
-  <si>
-    <t>0.044% (461.09)</t>
-  </si>
-  <si>
-    <t>0.049% (512.64)</t>
-  </si>
-  <si>
-    <t>0.027% (655.49)</t>
-  </si>
-  <si>
-    <t>0.027% (639.34)</t>
-  </si>
-  <si>
-    <t>0.032% (777.8)</t>
-  </si>
-  <si>
-    <t>0.091% (2169.87)</t>
-  </si>
-  <si>
-    <t>0.094% (2253.62)</t>
-  </si>
-  <si>
-    <t>0.102% (2447.19)</t>
-  </si>
-  <si>
-    <t>0.006% (363.15)</t>
-  </si>
-  <si>
-    <t>0.006% (350.34)</t>
-  </si>
-  <si>
-    <t>0.006% (396.34)</t>
-  </si>
-  <si>
-    <t>0.017% (1060.16)</t>
-  </si>
-  <si>
-    <t>0.016% (1036.91)</t>
-  </si>
-  <si>
-    <t>0.017% (1103.85)</t>
-  </si>
-  <si>
     <t>BMweights</t>
   </si>
   <si>
     <t>PDweights</t>
   </si>
   <si>
-    <t>All data shown here pertains to MSAs whose residues were masked at a threshold of 0.5</t>
+    <t>0.976% (43.25)</t>
+  </si>
+  <si>
+    <t>0.959% (42.49)</t>
+  </si>
+  <si>
+    <t>1.001% (44.35)</t>
+  </si>
+  <si>
+    <t>2.029% (89.32)</t>
+  </si>
+  <si>
+    <t>1.993% (87.69)</t>
+  </si>
+  <si>
+    <t>2.576% (113.67)</t>
+  </si>
+  <si>
+    <t>1.04% (107.75)</t>
+  </si>
+  <si>
+    <t>1.03% (106.73)</t>
+  </si>
+  <si>
+    <t>1.049% (108.67)</t>
+  </si>
+  <si>
+    <t>2.484% (256.84)</t>
+  </si>
+  <si>
+    <t>2.429% (251.01)</t>
+  </si>
+  <si>
+    <t>2.557% (264.28)</t>
+  </si>
+  <si>
+    <t>2.703% (653.38)</t>
+  </si>
+  <si>
+    <t>2.624% (634.76)</t>
+  </si>
+  <si>
+    <t>3.153% (762.93)</t>
+  </si>
+  <si>
+    <t>9.426% (2280.15)</t>
+  </si>
+  <si>
+    <t>9.623% (2326.67)</t>
+  </si>
+  <si>
+    <t>10.429% (2522.89)</t>
+  </si>
+  <si>
+    <t>0.599% (382.88)</t>
+  </si>
+  <si>
+    <t>0.573% (366.12)</t>
+  </si>
+  <si>
+    <t>0.648% (413.73)</t>
+  </si>
+  <si>
+    <t>1.755% (1126.08)</t>
+  </si>
+  <si>
+    <t>1.864% (1198.67)</t>
+  </si>
+  <si>
+    <t>1.937% (1245.29)</t>
+  </si>
+  <si>
+    <t>0.919% (40.56)</t>
+  </si>
+  <si>
+    <t>0.907% (40.01)</t>
+  </si>
+  <si>
+    <t>0.948% (41.82)</t>
+  </si>
+  <si>
+    <t>2.117% (93.1)</t>
+  </si>
+  <si>
+    <t>2.091% (91.96)</t>
+  </si>
+  <si>
+    <t>2.668% (117.72)</t>
+  </si>
+  <si>
+    <t>1.378% (143.81)</t>
+  </si>
+  <si>
+    <t>1.36% (141.86)</t>
+  </si>
+  <si>
+    <t>1.425% (148.7)</t>
+  </si>
+  <si>
+    <t>4.186% (435.8)</t>
+  </si>
+  <si>
+    <t>4.435% (461.09)</t>
+  </si>
+  <si>
+    <t>4.93% (512.64)</t>
+  </si>
+  <si>
+    <t>2.732% (655.49)</t>
+  </si>
+  <si>
+    <t>2.664% (639.34)</t>
+  </si>
+  <si>
+    <t>3.241% (777.8)</t>
+  </si>
+  <si>
+    <t>9.059% (2169.87)</t>
+  </si>
+  <si>
+    <t>9.416% (2253.62)</t>
+  </si>
+  <si>
+    <t>10.219% (2447.19)</t>
+  </si>
+  <si>
+    <t>0.572% (363.15)</t>
+  </si>
+  <si>
+    <t>0.551% (350.34)</t>
+  </si>
+  <si>
+    <t>0.624% (396.34)</t>
+  </si>
+  <si>
+    <t>1.671% (1060.16)</t>
+  </si>
+  <si>
+    <t>1.629% (1036.91)</t>
+  </si>
+  <si>
+    <t>1.739% (1103.85)</t>
+  </si>
+  <si>
+    <t>Percent Gaps</t>
+  </si>
+  <si>
+    <t>All data data concerning percent/number of sites masked shown here pertains to MSAs whose residues were masked at a threshold of 0.5</t>
+  </si>
+  <si>
+    <t>Note that masking does not influence the number of gaps in an alignment, so those numbers are held constant for a given simulation set.</t>
   </si>
 </sst>
 </file>
@@ -256,12 +253,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -269,10 +278,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -602,14 +624,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
@@ -619,7 +642,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -629,31 +652,31 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -663,26 +686,26 @@
       <c r="B3" s="1">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
+      <c r="C3" s="3">
+        <v>0.11899999999999999</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -690,28 +713,28 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -719,28 +742,28 @@
         <v>0</v>
       </c>
       <c r="B5" s="1">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -748,323 +771,154 @@
         <v>0</v>
       </c>
       <c r="B6" s="1">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>158</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.505</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>60</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.11600000000000001</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>60</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.313</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>158</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.58099999999999996</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
+        <v>158</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.48399999999999999</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1">
-        <v>60</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1">
-        <v>60</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1">
-        <v>158</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to supp tables
</commit_message>
<xml_diff>
--- a/Manuscript/Revision/TableS3.xlsx
+++ b/Manuscript/Revision/TableS3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>HA</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Note that masking does not influence the number of gaps in an alignment, so those numbers are held constant for a given simulation set.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Percent gaps were calculated from unfiltered alignments as the total number of gaps divided by the total number of MSA positions, and represent the percentage of columns with at least one gap, averaged across all MSA replicates.</t>
   </si>
 </sst>
 </file>
@@ -253,8 +256,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -275,12 +282,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -288,6 +295,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -295,6 +304,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -624,15 +635,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
@@ -641,14 +652,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
@@ -686,7 +697,7 @@
       <c r="B3" s="1">
         <v>11</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.11899999999999999</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -715,7 +726,7 @@
       <c r="B4" s="1">
         <v>26</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.26</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -744,7 +755,7 @@
       <c r="B5" s="1">
         <v>60</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.59399999999999997</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -773,7 +784,7 @@
       <c r="B6" s="1">
         <v>158</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>0.505</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -802,7 +813,7 @@
       <c r="B7" s="1">
         <v>11</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>0.11600000000000001</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -831,7 +842,7 @@
       <c r="B8" s="1">
         <v>26</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.313</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -860,7 +871,7 @@
       <c r="B9" s="1">
         <v>60</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>0.58099999999999996</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -889,7 +900,7 @@
       <c r="B10" s="1">
         <v>158</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0.48399999999999999</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -917,7 +928,12 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>